<commit_message>
removed differentiation between rod and shell nodes
</commit_message>
<xml_diff>
--- a/experiments/pneunet/nat_curve_new.xlsx
+++ b/experiments/pneunet/nat_curve_new.xlsx
@@ -160,7 +160,7 @@
         <v>-0.00012559911533028653</v>
       </c>
       <c r="C9" s="0">
-        <v>-0.00018811131932413812</v>
+        <v>-0.00018811131932414826</v>
       </c>
     </row>
     <row r="10">
@@ -171,7 +171,7 @@
         <v>0.0059802774310901592</v>
       </c>
       <c r="C10" s="0">
-        <v>0.0059557483833995459</v>
+        <v>0.0059557483833995416</v>
       </c>
     </row>
     <row r="11">
@@ -193,7 +193,7 @@
         <v>-0.0003762997162214164</v>
       </c>
       <c r="C12" s="0">
-        <v>-0.00056266436372444818</v>
+        <v>-0.00056266436372447821</v>
       </c>
     </row>
     <row r="13">
@@ -204,7 +204,7 @@
         <v>0.0079448427848444764</v>
       </c>
       <c r="C13" s="0">
-        <v>0.0078764257908553355</v>
+        <v>0.0078764257908553216</v>
       </c>
     </row>
     <row r="14">
@@ -226,7 +226,7 @@
         <v>-0.00075111040591529024</v>
       </c>
       <c r="C15" s="0">
-        <v>-0.0011203366863561201</v>
+        <v>-0.0011203366863561796</v>
       </c>
     </row>
     <row r="16">
@@ -237,7 +237,7 @@
         <v>0.0098819937814132973</v>
       </c>
       <c r="C16" s="0">
-        <v>0.009736138417838892</v>
+        <v>0.0097361384178388626</v>
       </c>
     </row>
     <row r="17">
@@ -259,7 +259,7 @@
         <v>-0.001248549973547983</v>
       </c>
       <c r="C18" s="0">
-        <v>-0.0018561825290256829</v>
+        <v>-0.0018561825290257805</v>
       </c>
     </row>
     <row r="19">
@@ -270,7 +270,7 @@
         <v>0.011784084324975144</v>
       </c>
       <c r="C19" s="0">
-        <v>0.011518399465300205</v>
+        <v>0.011518399465300153</v>
       </c>
     </row>
     <row r="20">
@@ -292,7 +292,7 @@
         <v>-0.0018666532773741972</v>
       </c>
       <c r="C21" s="0">
-        <v>-0.0027636767445299686</v>
+        <v>-0.0027636767445301117</v>
       </c>
     </row>
     <row r="22">
@@ -303,7 +303,7 @@
         <v>0.01364360698708408</v>
       </c>
       <c r="C22" s="0">
-        <v>0.013207409133359325</v>
+        <v>0.01320740913335924</v>
       </c>
     </row>
     <row r="23">
@@ -325,7 +325,7 @@
         <v>-0.0026029790346151502</v>
       </c>
       <c r="C24" s="0">
-        <v>-0.0038347727084520758</v>
+        <v>-0.0038347727084522714</v>
       </c>
     </row>
     <row r="25">
@@ -336,7 +336,7 @@
         <v>0.01545322261252745</v>
       </c>
       <c r="C25" s="0">
-        <v>0.014788194623862001</v>
+        <v>0.014788194623861873</v>
       </c>
     </row>
     <row r="26">
@@ -358,7 +358,7 @@
         <v>-0.003454619486766852</v>
       </c>
       <c r="C27" s="0">
-        <v>-0.0050599737053268938</v>
+        <v>-0.0050599737053271462</v>
       </c>
     </row>
     <row r="28">
@@ -369,7 +369,7 @@
         <v>0.017205789258144786</v>
       </c>
       <c r="C28" s="0">
-        <v>0.016246742805349667</v>
+        <v>0.01624674280534948</v>
       </c>
     </row>
     <row r="29">
@@ -391,7 +391,7 @@
         <v>-0.0044182119018887312</v>
       </c>
       <c r="C30" s="0">
-        <v>-0.0064284171552421686</v>
+        <v>-0.0064284171552424817</v>
       </c>
     </row>
     <row r="31">
@@ -402,7 +402,7 @@
         <v>0.018894390351015641</v>
       </c>
       <c r="C31" s="0">
-        <v>0.017570124367443912</v>
+        <v>0.017570124367443655</v>
       </c>
     </row>
     <row r="32">
@@ -424,7 +424,7 @@
         <v>-0.0054899518682305706</v>
       </c>
       <c r="C33" s="0">
-        <v>-0.0079279709337302818</v>
+        <v>-0.0079279709337306565</v>
       </c>
     </row>
     <row r="34">
@@ -435,7 +435,7 @@
         <v>0.020512361955519719</v>
       </c>
       <c r="C34" s="0">
-        <v>0.018746608367050856</v>
+        <v>0.018746608367050516</v>
       </c>
     </row>
     <row r="35">
@@ -457,7 +457,7 @@
         <v>-0.006665608326575226</v>
       </c>
       <c r="C36" s="0">
-        <v>-0.0095453409312096765</v>
+        <v>-0.0095453409312101119</v>
       </c>
     </row>
     <row r="37">
@@ -468,7 +468,7 @@
         <v>0.022053319042292064</v>
       </c>
       <c r="C37" s="0">
-        <v>0.019765766153809729</v>
+        <v>0.019765766153809292</v>
       </c>
     </row>
     <row r="38">
@@ -490,7 +490,7 @@
         <v>-0.0079405402819015727</v>
       </c>
       <c r="C39" s="0">
-        <v>-0.011266188899174828</v>
+        <v>-0.011266188899175321</v>
       </c>
     </row>
     <row r="40">
@@ -501,7 +501,7 @@
         <v>0.023511180656025376</v>
       </c>
       <c r="C40" s="0">
-        <v>0.020618563756099426</v>
+        <v>0.020618563756098877</v>
       </c>
     </row>
     <row r="41">
@@ -523,7 +523,7 @@
         <v>-0.0093097151284313433</v>
       </c>
       <c r="C42" s="0">
-        <v>-0.01307525953966622</v>
+        <v>-0.013075259539666765</v>
       </c>
     </row>
     <row r="43">
@@ -534,7 +534,7 @@
         <v>0.024880193883396341</v>
       </c>
       <c r="C43" s="0">
-        <v>0.021297441910859242</v>
+        <v>0.021297441910858566</v>
       </c>
     </row>
     <row r="44">
@@ -556,7 +556,7 @@
         <v>-0.010767728515839649</v>
       </c>
       <c r="C45" s="0">
-        <v>-0.014956515713062521</v>
+        <v>-0.014956515713063112</v>
       </c>
     </row>
     <row r="46">
@@ -567,7 +567,7 @@
         <v>0.026154956527096148</v>
       </c>
       <c r="C46" s="0">
-        <v>0.021796383029588841</v>
+        <v>0.021796383029588026</v>
       </c>
     </row>
     <row r="47">
@@ -589,7 +589,7 @@
         <v>-0.012308825678404717</v>
       </c>
       <c r="C48" s="0">
-        <v>-0.016893280567632805</v>
+        <v>-0.016893280567633433</v>
       </c>
     </row>
     <row r="49">
@@ -600,7 +600,7 @@
         <v>0.027330438397010302</v>
       </c>
       <c r="C49" s="0">
-        <v>0.022110964508221111</v>
+        <v>0.02211096450822014</v>
       </c>
     </row>
     <row r="50">
@@ -622,7 +622,7 @@
         <v>-0.013926924143170857</v>
       </c>
       <c r="C51" s="0">
-        <v>-0.018868385333191538</v>
+        <v>-0.018868385333192191</v>
       </c>
     </row>
     <row r="52">
@@ -633,7 +633,7 @@
         <v>0.028402001134999671</v>
       </c>
       <c r="C52" s="0">
-        <v>0.022238397909108261</v>
+        <v>0.022238397909107123</v>
       </c>
     </row>
     <row r="53">
@@ -655,7 +655,7 @@
         <v>-0.015615637727820302</v>
       </c>
       <c r="C54" s="0">
-        <v>-0.020864321471147269</v>
+        <v>-0.020864321471147931</v>
       </c>
     </row>
     <row r="55">
@@ -666,7 +666,7 @@
         <v>0.029365416495464276</v>
       </c>
       <c r="C55" s="0">
-        <v>0.022177553668080382</v>
+        <v>0.022177553668079067</v>
       </c>
     </row>
     <row r="56">
@@ -688,7 +688,7 @@
         <v>-0.017368301733915407</v>
       </c>
       <c r="C57" s="0">
-        <v>-0.022863395834669665</v>
+        <v>-0.022863395834670324</v>
       </c>
     </row>
     <row r="58">
@@ -699,7 +699,7 @@
         <v>0.030216883009901559</v>
       </c>
       <c r="C58" s="0">
-        <v>0.021928971107341981</v>
+        <v>0.021928971107340482</v>
       </c>
     </row>
     <row r="59">
@@ -721,7 +721,7 @@
         <v>-0.019177999236501184</v>
       </c>
       <c r="C60" s="0">
-        <v>-0.024847887465962084</v>
+        <v>-0.024847887465962722</v>
       </c>
     </row>
     <row r="61">
@@ -732,7 +732,7 @@
         <v>0.030953040969979754</v>
       </c>
       <c r="C61" s="0">
-        <v>0.021494853664753955</v>
+        <v>0.021494853664752261</v>
       </c>
     </row>
     <row r="62">
@@ -754,7 +754,7 @@
         <v>-0.021037588366767255</v>
       </c>
       <c r="C63" s="0">
-        <v>-0.026800204642961907</v>
+        <v>-0.0268002046429625</v>
       </c>
     </row>
     <row r="64">
@@ -765,7 +765,7 @@
         <v>0.031570985670211507</v>
       </c>
       <c r="C64" s="0">
-        <v>0.020879049380673233</v>
+        <v>0.020879049380671338</v>
       </c>
     </row>
     <row r="65">
@@ -787,7 +787,7 @@
         <v>-0.022939730480574915</v>
       </c>
       <c r="C66" s="0">
-        <v>-0.02870304078533888</v>
+        <v>-0.028703040785339407</v>
       </c>
     </row>
     <row r="67">
@@ -798,7 +798,7 @@
         <v>0.032068278858107743</v>
       </c>
       <c r="C67" s="0">
-        <v>0.020087016813848314</v>
+        <v>0.020087016813846222</v>
       </c>
     </row>
     <row r="68">
@@ -820,7 +820,7 @@
         <v>-0.024876919102173559</v>
       </c>
       <c r="C69" s="0">
-        <v>-0.030539527839457074</v>
+        <v>-0.030539527839457514</v>
       </c>
     </row>
     <row r="70">
@@ -831,7 +831,7 @@
         <v>0.032442958346692634</v>
       </c>
       <c r="C70" s="0">
-        <v>0.019125776686752877</v>
+        <v>0.019125776686750584</v>
       </c>
     </row>
     <row r="71">
@@ -853,7 +853,7 @@
         <v>-0.02684150952937572</v>
       </c>
       <c r="C72" s="0">
-        <v>-0.032293385783938935</v>
+        <v>-0.032293385783939262</v>
       </c>
     </row>
     <row r="73">
@@ -864,7 +864,7 @@
         <v>0.032693545751440685</v>
       </c>
       <c r="C73" s="0">
-        <v>0.018003849687047928</v>
+        <v>0.018003849687045437</v>
       </c>
     </row>
     <row r="74">
@@ -886,7 +886,7 @@
         <v>-0.028825748983843172</v>
       </c>
       <c r="C75" s="0">
-        <v>-0.033949066931442722</v>
+        <v>-0.033949066931442923</v>
       </c>
     </row>
     <row r="76">
@@ -897,7 +897,7 @@
         <v>0.032819052321029704</v>
       </c>
       <c r="C76" s="0">
-        <v>0.016731180974481067</v>
+        <v>0.016731180974478382</v>
       </c>
     </row>
     <row r="77">
@@ -919,7 +919,7 @@
         <v>-0.030821807187969164</v>
       </c>
       <c r="C78" s="0">
-        <v>-0.035491893747956124</v>
+        <v>-0.035491893747956159</v>
       </c>
     </row>
     <row r="79">
@@ -930,7 +930,7 @@
         <v>0.03281898283876087</v>
       </c>
       <c r="C79" s="0">
-        <v>0.01531905206037289</v>
+        <v>0.015319052060370018</v>
       </c>
     </row>
     <row r="80">
@@ -952,7 +952,7 @@
         <v>-0.03282180724813244</v>
       </c>
       <c r="C81" s="0">
-        <v>-0.036908188967932146</v>
+        <v>-0.036908188967932</v>
       </c>
     </row>
     <row r="82">
@@ -963,7 +963,7 @@
         <v>0.032693337579051886</v>
       </c>
       <c r="C82" s="0">
-        <v>0.013779980838858384</v>
+        <v>0.013779980838855338</v>
       </c>
     </row>
     <row r="83">
@@ -985,7 +985,7 @@
         <v>-0.034817856722855582</v>
       </c>
       <c r="C84" s="0">
-        <v>-0.038185396851463459</v>
+        <v>-0.038185396851463105</v>
       </c>
     </row>
     <row r="85">
@@ -996,7 +996,7 @@
         <v>0.03244261231103128</v>
       </c>
       <c r="C85" s="0">
-        <v>0.012127610654245643</v>
+        <v>0.012127610654242437</v>
       </c>
     </row>
     <row r="86">
@@ -1018,7 +1018,7 @@
         <v>-0.036802078753628543</v>
       </c>
       <c r="C87" s="0">
-        <v>-0.039312194507822321</v>
+        <v>-0.039312194507821731</v>
       </c>
     </row>
     <row r="88">
@@ -1029,7 +1029,7 @@
         <v>0.032067796348923358</v>
       </c>
       <c r="C88" s="0">
-        <v>0.010376589386282954</v>
+        <v>0.010376589386279606</v>
       </c>
     </row>
     <row r="89">
@@ -1051,7 +1051,7 @@
         <v>-0.038766643135862595</v>
       </c>
       <c r="C90" s="0">
-        <v>-0.04027859229741064</v>
+        <v>-0.040278592297409786</v>
       </c>
     </row>
     <row r="91">
@@ -1062,7 +1062,7 @@
         <v>0.03157036865658415</v>
       </c>
       <c r="C91" s="0">
-        <v>0.0085424396239118638</v>
+        <v>0.0085424396239083943</v>
       </c>
     </row>
     <row r="92">
@@ -1084,7 +1084,7 @@
         <v>-0.040703797207622613</v>
       </c>
       <c r="C93" s="0">
-        <v>-0.041076022420702248</v>
+        <v>-0.041076022420701123</v>
       </c>
     </row>
     <row r="94">
@@ -1095,7 +1095,7 @@
         <v>0.030952292021198795</v>
       </c>
       <c r="C94" s="0">
-        <v>0.0066414210774222082</v>
+        <v>0.0066414210774186399</v>
       </c>
     </row>
     <row r="95">
@@ -1117,7 +1117,7 @@
         <v>-0.042605896434446844</v>
       </c>
       <c r="C96" s="0">
-        <v>-0.04169741490727441</v>
+        <v>-0.041697414907272988</v>
       </c>
     </row>
     <row r="97">
@@ -1128,7 +1128,7 @@
         <v>0.030216005318751463</v>
       </c>
       <c r="C97" s="0">
-        <v>0.0046903864480826981</v>
+        <v>0.0046903864480790586</v>
       </c>
     </row>
     <row r="98">
@@ -1150,7 +1150,7 @@
         <v>-0.044465434569702388</v>
       </c>
       <c r="C99" s="0">
-        <v>-0.042137260329595964</v>
+        <v>-0.042137260329594223</v>
       </c>
     </row>
     <row r="100">
@@ -1161,7 +1161,7 @@
         <v>0.029364413901399086</v>
       </c>
       <c r="C100" s="0">
-        <v>0.0027066320326256145</v>
+        <v>0.0027066320326219325</v>
       </c>
     </row>
     <row r="101">
@@ -1183,7 +1183,7 @@
         <v>-0.046275073271538063</v>
       </c>
       <c r="C102" s="0">
-        <v>-0.042391658683870716</v>
+        <v>-0.042391658683868641</v>
       </c>
     </row>
     <row r="103">
@@ -1194,7 +1194,7 @@
         <v>0.028400878144291181</v>
       </c>
       <c r="C103" s="0">
-        <v>0.00070774438678248555</v>
+        <v>0.00070774438677879135</v>
       </c>
     </row>
     <row r="104">
@@ -1216,7 +1216,7 @@
         <v>-0.048027671059579065</v>
       </c>
       <c r="C105" s="0">
-        <v>-0.042458354002836103</v>
+        <v>-0.042458354002833681</v>
       </c>
     </row>
     <row r="106">
@@ -1227,7 +1227,7 @@
         <v>0.027329200196649733</v>
       </c>
       <c r="C106" s="0">
-        <v>-0.0012885555932327195</v>
+        <v>-0.0012885555932363921</v>
       </c>
     </row>
     <row r="107">
@@ -1249,7 +1249,7 @@
         <v>-0.049716311497053217</v>
       </c>
       <c r="C108" s="0">
-        <v>-0.042336754391750255</v>
+        <v>-0.042336754391747479</v>
       </c>
     </row>
     <row r="109">
@@ -1260,7 +1260,7 @@
         <v>0.026153608989026848</v>
       </c>
       <c r="C109" s="0">
-        <v>-0.0032645697904359018</v>
+        <v>-0.0032645697904395174</v>
       </c>
     </row>
     <row r="110">
@@ -1282,7 +1282,7 @@
         <v>-0.051334330487038102</v>
       </c>
       <c r="C111" s="0">
-        <v>-0.042027937307369957</v>
+        <v>-0.042027937307366814</v>
       </c>
     </row>
     <row r="112">
@@ -1293,7 +1293,7 @@
         <v>0.024878743555564711</v>
       </c>
       <c r="C112" s="0">
-        <v>-0.0052027797983688192</v>
+        <v>-0.0052027797983723407</v>
       </c>
     </row>
     <row r="113">
@@ -1315,7 +1315,7 @@
         <v>-0.052875342574960391</v>
       </c>
       <c r="C114" s="0">
-        <v>-0.041534640028663521</v>
+        <v>-0.04153464002866001</v>
       </c>
     </row>
     <row r="115">
@@ -1326,7 +1326,7 @@
         <v>0.023509634736764793</v>
       </c>
       <c r="C115" s="0">
-        <v>-0.00708600227875315</v>
+        <v>-0.0070860022787565397</v>
       </c>
     </row>
     <row r="116">
@@ -1348,7 +1348,7 @@
         <v>-0.054333266153352114</v>
       </c>
       <c r="C117" s="0">
-        <v>-0.04086123539511919</v>
+        <v>-0.040861235395115311</v>
       </c>
     </row>
     <row r="118">
@@ -1359,7 +1359,7 @@
         <v>0.022051685334703086</v>
       </c>
       <c r="C118" s="0">
-        <v>-0.0088975413767012051</v>
+        <v>-0.008897541376704423</v>
       </c>
     </row>
     <row r="119">
@@ -1381,7 +1381,7 @@
         <v>-0.055702347469158295</v>
       </c>
       <c r="C120" s="0">
-        <v>-0.040013693011699165</v>
+        <v>-0.040013693011694933</v>
       </c>
     </row>
     <row r="121">
@@ -1392,7 +1392,7 @@
         <v>0.02051064879878026</v>
       </c>
       <c r="C121" s="0">
-        <v>-0.010621336850783087</v>
+        <v>-0.010621336850786091</v>
       </c>
     </row>
     <row r="122">
@@ -1414,7 +1414,7 @@
         <v>-0.056977183338579894</v>
       </c>
       <c r="C123" s="0">
-        <v>-0.038999526237650073</v>
+        <v>-0.038999526237645486</v>
       </c>
     </row>
     <row r="124">
@@ -1425,7 +1425,7 @@
         <v>0.018892606525943482</v>
       </c>
       <c r="C124" s="0">
-        <v>-0.012242106608066242</v>
+        <v>-0.01224210660806899</v>
       </c>
     </row>
     <row r="125">
@@ -1447,7 +1447,7 @@
         <v>-0.058152742479508891</v>
       </c>
       <c r="C126" s="0">
-        <v>-0.037827725390406707</v>
+        <v>-0.037827725390401787</v>
       </c>
     </row>
     <row r="127">
@@ -1458,7 +1458,7 @@
         <v>0.017203943864836591</v>
       </c>
       <c r="C127" s="0">
-        <v>-0.013745482371802203</v>
+        <v>-0.013745482371804655</v>
       </c>
     </row>
     <row r="128">
@@ -1480,7 +1480,7 @@
         <v>-0.059224385377047342</v>
       </c>
       <c r="C129" s="0">
-        <v>-0.03650867770886141</v>
+        <v>-0.036508677708856178</v>
       </c>
     </row>
     <row r="130">
@@ -1491,7 +1491,7 @@
         <v>0.015451324918504291</v>
       </c>
       <c r="C130" s="0">
-        <v>-0.015118137252385666</v>
+        <v>-0.015118137252387774</v>
       </c>
     </row>
     <row r="131">
@@ -1513,7 +1513,7 @@
         <v>-0.060187882603379754</v>
       </c>
       <c r="C132" s="0">
-        <v>-0.035054074736451425</v>
+        <v>-0.035054074736445909</v>
       </c>
     </row>
     <row r="133">
@@ -1524,7 +1524,7 @@
         <v>0.013641666245072261</v>
       </c>
       <c r="C133" s="0">
-        <v>-0.016347904043452606</v>
+        <v>-0.01634790404345433</v>
       </c>
     </row>
     <row r="134">
@@ -1546,7 +1546,7 @@
         <v>-0.061039431519364362</v>
       </c>
       <c r="C135" s="0">
-        <v>-0.033476807906235848</v>
+        <v>-0.033476807906230081</v>
       </c>
     </row>
     <row r="136">
@@ -1557,7 +1557,7 @@
         <v>0.011782109560229291</v>
       </c>
       <c r="C136" s="0">
-        <v>-0.017423883123660971</v>
+        <v>-0.017423883123662262</v>
       </c>
     </row>
     <row r="137">
@@ -1579,7 +1579,7 @@
         <v>-0.061775671291600137</v>
       </c>
       <c r="C138" s="0">
-        <v>-0.031790853235836684</v>
+        <v>-0.031790853235830717</v>
       </c>
     </row>
     <row r="139">
@@ -1590,7 +1590,7 @@
         <v>0.0098799935493311241</v>
       </c>
       <c r="C139" s="0">
-        <v>-0.018336538886226782</v>
+        <v>-0.018336538886227598</v>
       </c>
     </row>
     <row r="140">
@@ -1612,7 +1612,7 @@
         <v>-0.062393696165387438</v>
       </c>
       <c r="C141" s="0">
-        <v>-0.030011146174073466</v>
+        <v>-0.030011146174067339</v>
       </c>
     </row>
     <row r="142">
@@ -1623,7 +1623,7 @@
         <v>0.0079428249005152832</v>
       </c>
       <c r="C142" s="0">
-        <v>-0.019077783536151593</v>
+        <v>-0.019077783536151884</v>
       </c>
     </row>
     <row r="143">
@@ -1645,7 +1645,7 @@
         <v>-0.062891066940904045</v>
       </c>
       <c r="C144" s="0">
-        <v>-0.028153447883794286</v>
+        <v>-0.028153447883788062</v>
       </c>
     </row>
     <row r="145">
@@ -1656,7 +1656,7 @@
         <v>0.0059782486733487867</v>
       </c>
       <c r="C145" s="0">
-        <v>-0.019641046560092631</v>
+        <v>-0.01964104656009235</v>
       </c>
     </row>
     <row r="146">
@@ -1678,7 +1678,7 @@
         <v>-0.063265820607038892</v>
       </c>
       <c r="C147" s="0">
-        <v>-0.026234205305769275</v>
+        <v>-0.02623420530576303</v>
       </c>
     </row>
     <row r="148">
@@ -1689,7 +1689,7 @@
         <v>0.0039940181202122761</v>
       </c>
       <c r="C148" s="0">
-        <v>-0.020021326807962071</v>
+        <v>-0.02002132680796118</v>
       </c>
     </row>
     <row r="149">
@@ -1711,7 +1711,7 @@
         <v>-0.063516478094638396</v>
       </c>
       <c r="C150" s="0">
-        <v>-0.024270412026891463</v>
+        <v>-0.024270412026885273</v>
       </c>
     </row>
     <row r="151">
@@ -1722,7 +1722,7 @@
         <v>0.0019979640797892148</v>
       </c>
       <c r="C151" s="0">
-        <v>-0.020215225623614906</v>
+        <v>-0.020215225623613383</v>
       </c>
     </row>
     <row r="152">
@@ -1744,7 +1744,7 @@
         <v>-0.063642050118400767</v>
       </c>
       <c r="C153" s="0">
-        <v>-0.022279485554475138</v>
+        <v>-0.02227948555446908</v>
       </c>
     </row>
     <row r="154">

</xml_diff>